<commit_message>
OW-969,recorded test results under different asset amount scenarios and time limits
</commit_message>
<xml_diff>
--- a/test/testAssetAmount/assetAmountPerformance.xlsx
+++ b/test/testAssetAmount/assetAmountPerformance.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="107">
   <si>
     <t>RData</t>
   </si>
@@ -304,6 +304,42 @@
   </si>
   <si>
     <t>10.3699999999953</t>
+  </si>
+  <si>
+    <t>10.5100000000093</t>
+  </si>
+  <si>
+    <t>40.3500000000058</t>
+  </si>
+  <si>
+    <t>160.360000000015</t>
+  </si>
+  <si>
+    <t>250.359999999986</t>
+  </si>
+  <si>
+    <t>14.2099999999919</t>
+  </si>
+  <si>
+    <t>16.3000000000175</t>
+  </si>
+  <si>
+    <t>15.4700000000012</t>
+  </si>
+  <si>
+    <t>14.6199999999953</t>
+  </si>
+  <si>
+    <t>10.429999999993</t>
+  </si>
+  <si>
+    <t>90.390000000014</t>
+  </si>
+  <si>
+    <t>160.389999999985</t>
+  </si>
+  <si>
+    <t>175.929999999993</t>
   </si>
 </sst>
 </file>
@@ -369,7 +405,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="416">
+  <cellXfs count="502">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
       <alignment wrapText="1"/>
@@ -1608,6 +1644,264 @@
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
@@ -1901,10 +2195,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2496,7 +2790,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40">
+    <row ht="30" r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="162" t="s">
         <v>5</v>
       </c>
@@ -2516,7 +2810,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41">
+    <row ht="30" r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="168" t="s">
         <v>2</v>
       </c>
@@ -2536,7 +2830,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="42">
+    <row ht="30" r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="174" t="s">
         <v>2</v>
       </c>
@@ -2556,7 +2850,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="43">
+    <row ht="30" r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="180" t="s">
         <v>2</v>
       </c>
@@ -2576,7 +2870,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="44">
+    <row ht="30" r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="186" t="s">
         <v>2</v>
       </c>
@@ -2596,7 +2890,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="45">
+    <row ht="30" r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="192" t="s">
         <v>2</v>
       </c>
@@ -2616,7 +2910,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="46">
+    <row ht="30" r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="198" t="s">
         <v>5</v>
       </c>
@@ -2636,7 +2930,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="47">
+    <row ht="30" r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="204" t="s">
         <v>5</v>
       </c>
@@ -2656,7 +2950,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="48">
+    <row ht="30" r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="210" t="s">
         <v>5</v>
       </c>
@@ -2676,7 +2970,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="49">
+    <row ht="30" r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="216" t="s">
         <v>5</v>
       </c>
@@ -2696,7 +2990,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50">
+    <row ht="30" r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="222" t="s">
         <v>5</v>
       </c>
@@ -2716,7 +3010,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="51">
+    <row ht="30" r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="228" t="s">
         <v>5</v>
       </c>
@@ -2736,7 +3030,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="52">
+    <row ht="30" r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="234" t="s">
         <v>5</v>
       </c>
@@ -2756,7 +3050,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="53">
+    <row ht="30" r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="240" t="s">
         <v>5</v>
       </c>
@@ -2776,7 +3070,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="54">
+    <row ht="30" r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="246" t="s">
         <v>5</v>
       </c>
@@ -2796,7 +3090,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="55">
+    <row ht="30" r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="252" t="s">
         <v>5</v>
       </c>
@@ -2816,7 +3110,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="56">
+    <row ht="30" r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="258" t="s">
         <v>4</v>
       </c>
@@ -2836,7 +3130,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="57">
+    <row ht="30" r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="264" t="s">
         <v>4</v>
       </c>
@@ -2856,7 +3150,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="58">
+    <row ht="30" r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="270" t="s">
         <v>4</v>
       </c>
@@ -2876,7 +3170,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="59">
+    <row ht="30" r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="276" t="s">
         <v>4</v>
       </c>
@@ -2896,7 +3190,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="60">
+    <row ht="30" r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="282" t="s">
         <v>4</v>
       </c>
@@ -2916,7 +3210,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="61">
+    <row ht="30" r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="288" t="s">
         <v>6</v>
       </c>
@@ -2924,7 +3218,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="62">
+    <row ht="30" r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="290" t="s">
         <v>7</v>
       </c>
@@ -2932,7 +3226,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="63">
+    <row ht="30" r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="292" t="s">
         <v>2</v>
       </c>
@@ -2952,7 +3246,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="64">
+    <row ht="30" r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="298" t="s">
         <v>2</v>
       </c>
@@ -2972,7 +3266,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="65">
+    <row ht="30" r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="304" t="s">
         <v>2</v>
       </c>
@@ -2992,7 +3286,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="66">
+    <row ht="30" r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="310" t="s">
         <v>2</v>
       </c>
@@ -3012,7 +3306,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="67">
+    <row ht="30" r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="316" t="s">
         <v>2</v>
       </c>
@@ -3032,7 +3326,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="68">
+    <row ht="30" r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="322" t="s">
         <v>5</v>
       </c>
@@ -3052,7 +3346,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="69">
+    <row ht="30" r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="328" t="s">
         <v>5</v>
       </c>
@@ -3072,7 +3366,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="70">
+    <row ht="30" r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="334" t="s">
         <v>5</v>
       </c>
@@ -3092,7 +3386,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="71">
+    <row ht="30" r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="340" t="s">
         <v>5</v>
       </c>
@@ -3112,7 +3406,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="72">
+    <row ht="30" r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="346" t="s">
         <v>5</v>
       </c>
@@ -3132,7 +3426,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="73">
+    <row ht="30" r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="352" t="s">
         <v>5</v>
       </c>
@@ -3152,7 +3446,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="74">
+    <row ht="30" r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="358" t="s">
         <v>5</v>
       </c>
@@ -3172,7 +3466,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="75">
+    <row ht="30" r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="364" t="s">
         <v>5</v>
       </c>
@@ -3192,7 +3486,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="76">
+    <row ht="30" r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="370" t="s">
         <v>5</v>
       </c>
@@ -3212,7 +3506,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="77">
+    <row ht="30" r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="376" t="s">
         <v>5</v>
       </c>
@@ -3232,7 +3526,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="78">
+    <row ht="30" r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="382" t="s">
         <v>4</v>
       </c>
@@ -3252,7 +3546,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="79">
+    <row ht="30" r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="388" t="s">
         <v>4</v>
       </c>
@@ -3272,7 +3566,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="80">
+    <row ht="30" r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="394" t="s">
         <v>4</v>
       </c>
@@ -3292,7 +3586,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="81">
+    <row ht="30" r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="400" t="s">
         <v>4</v>
       </c>
@@ -3312,7 +3606,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="82">
+    <row ht="30" r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="406" t="s">
         <v>4</v>
       </c>
@@ -3332,7 +3626,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="83">
+    <row ht="30" r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="412" t="s">
         <v>6</v>
       </c>
@@ -3340,12 +3634,312 @@
         <v>93</v>
       </c>
     </row>
-    <row r="84">
-      <c r="A84" t="s" s="414">
+    <row ht="30" r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="414" t="s">
         <v>7</v>
       </c>
-      <c r="B84" t="s" s="415">
+      <c r="B84" s="415" t="s">
         <v>94</v>
+      </c>
+    </row>
+    <row ht="30" r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="416" t="s">
+        <v>3</v>
+      </c>
+      <c r="B85" s="417" t="s">
+        <v>19</v>
+      </c>
+      <c r="C85" s="418" t="s">
+        <v>95</v>
+      </c>
+      <c r="D85" s="419" t="s">
+        <v>62</v>
+      </c>
+      <c r="E85" s="420" t="s">
+        <v>63</v>
+      </c>
+      <c r="F85" s="421" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row ht="30" r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="441" t="s">
+        <v>3</v>
+      </c>
+      <c r="B86" s="422" t="s">
+        <v>21</v>
+      </c>
+      <c r="C86" s="423" t="s">
+        <v>96</v>
+      </c>
+      <c r="D86" s="424" t="s">
+        <v>62</v>
+      </c>
+      <c r="E86" s="425" t="s">
+        <v>63</v>
+      </c>
+      <c r="F86" s="426" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row ht="30" r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="441" t="s">
+        <v>3</v>
+      </c>
+      <c r="B87" s="427" t="s">
+        <v>23</v>
+      </c>
+      <c r="C87" s="428" t="s">
+        <v>36</v>
+      </c>
+      <c r="D87" s="429" t="s">
+        <v>62</v>
+      </c>
+      <c r="E87" s="430" t="s">
+        <v>63</v>
+      </c>
+      <c r="F87" s="431" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row ht="30" r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="441" t="s">
+        <v>3</v>
+      </c>
+      <c r="B88" s="432" t="s">
+        <v>25</v>
+      </c>
+      <c r="C88" s="433" t="s">
+        <v>97</v>
+      </c>
+      <c r="D88" s="434" t="s">
+        <v>62</v>
+      </c>
+      <c r="E88" s="435" t="s">
+        <v>63</v>
+      </c>
+      <c r="F88" s="436" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row ht="30" r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="441" t="s">
+        <v>3</v>
+      </c>
+      <c r="B89" s="437" t="s">
+        <v>27</v>
+      </c>
+      <c r="C89" s="438" t="s">
+        <v>98</v>
+      </c>
+      <c r="D89" s="439" t="s">
+        <v>62</v>
+      </c>
+      <c r="E89" s="440" t="s">
+        <v>63</v>
+      </c>
+      <c r="F89" s="441" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="442" t="s">
+        <v>2</v>
+      </c>
+      <c r="B90" s="443" t="s">
+        <v>19</v>
+      </c>
+      <c r="C90" s="444" t="s">
+        <v>11</v>
+      </c>
+      <c r="D90" s="445" t="s">
+        <v>47</v>
+      </c>
+      <c r="E90" s="446" t="s">
+        <v>48</v>
+      </c>
+      <c r="F90" s="447" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="448" t="s">
+        <v>2</v>
+      </c>
+      <c r="B91" s="449" t="s">
+        <v>21</v>
+      </c>
+      <c r="C91" s="450" t="s">
+        <v>99</v>
+      </c>
+      <c r="D91" s="451" t="s">
+        <v>47</v>
+      </c>
+      <c r="E91" s="452" t="s">
+        <v>48</v>
+      </c>
+      <c r="F91" s="453" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="454" t="s">
+        <v>2</v>
+      </c>
+      <c r="B92" s="455" t="s">
+        <v>23</v>
+      </c>
+      <c r="C92" s="456" t="s">
+        <v>100</v>
+      </c>
+      <c r="D92" s="457" t="s">
+        <v>47</v>
+      </c>
+      <c r="E92" s="458" t="s">
+        <v>48</v>
+      </c>
+      <c r="F92" s="459" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="460" t="s">
+        <v>2</v>
+      </c>
+      <c r="B93" s="461" t="s">
+        <v>25</v>
+      </c>
+      <c r="C93" s="462" t="s">
+        <v>101</v>
+      </c>
+      <c r="D93" s="463" t="s">
+        <v>47</v>
+      </c>
+      <c r="E93" s="464" t="s">
+        <v>48</v>
+      </c>
+      <c r="F93" s="465" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="466" t="s">
+        <v>2</v>
+      </c>
+      <c r="B94" s="467" t="s">
+        <v>27</v>
+      </c>
+      <c r="C94" s="468" t="s">
+        <v>102</v>
+      </c>
+      <c r="D94" s="469" t="s">
+        <v>47</v>
+      </c>
+      <c r="E94" s="470" t="s">
+        <v>48</v>
+      </c>
+      <c r="F94" s="471" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="472" t="s">
+        <v>5</v>
+      </c>
+      <c r="B95" s="473" t="s">
+        <v>19</v>
+      </c>
+      <c r="C95" s="474" t="s">
+        <v>103</v>
+      </c>
+      <c r="D95" s="475" t="s">
+        <v>44</v>
+      </c>
+      <c r="E95" s="476" t="s">
+        <v>45</v>
+      </c>
+      <c r="F95" s="477" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="478" t="s">
+        <v>5</v>
+      </c>
+      <c r="B96" s="479" t="s">
+        <v>21</v>
+      </c>
+      <c r="C96" s="480" t="s">
+        <v>31</v>
+      </c>
+      <c r="D96" s="481" t="s">
+        <v>55</v>
+      </c>
+      <c r="E96" s="482" t="s">
+        <v>56</v>
+      </c>
+      <c r="F96" s="483" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="484" t="s">
+        <v>5</v>
+      </c>
+      <c r="B97" s="485" t="s">
+        <v>23</v>
+      </c>
+      <c r="C97" s="486" t="s">
+        <v>104</v>
+      </c>
+      <c r="D97" s="487" t="s">
+        <v>55</v>
+      </c>
+      <c r="E97" s="488" t="s">
+        <v>56</v>
+      </c>
+      <c r="F97" s="489" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="490" t="s">
+        <v>5</v>
+      </c>
+      <c r="B98" s="491" t="s">
+        <v>25</v>
+      </c>
+      <c r="C98" s="492" t="s">
+        <v>105</v>
+      </c>
+      <c r="D98" s="493" t="s">
+        <v>59</v>
+      </c>
+      <c r="E98" s="494" t="s">
+        <v>60</v>
+      </c>
+      <c r="F98" s="495" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s" s="496">
+        <v>5</v>
+      </c>
+      <c r="B99" t="s" s="497">
+        <v>27</v>
+      </c>
+      <c r="C99" t="s" s="498">
+        <v>106</v>
+      </c>
+      <c r="D99" t="s" s="499">
+        <v>59</v>
+      </c>
+      <c r="E99" t="s" s="500">
+        <v>60</v>
+      </c>
+      <c r="F99" t="s" s="501">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>